<commit_message>
Chg: Updated JTL and added remaining targets. Added remaining targets to combatflite file. Added .miz for target production
</commit_message>
<xml_diff>
--- a/INTELLIGENCE/TGT_LIST/OPAR v2.0_JOINT_TARGET_LIST_v1.2.xlsx
+++ b/INTELLIGENCE/TGT_LIST/OPAR v2.0_JOINT_TARGET_LIST_v1.2.xlsx
@@ -2277,9 +2277,6 @@
     <t>SYTGT135</t>
   </si>
   <si>
-    <t>Current as of: Version 1.1</t>
-  </si>
-  <si>
     <t>N36 02.682</t>
   </si>
   <si>
@@ -2320,6 +2317,9 @@
   </si>
   <si>
     <t>Backup ADCC</t>
+  </si>
+  <si>
+    <t>Current as of: Version 1.2</t>
   </si>
 </sst>
 </file>
@@ -2948,11 +2948,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2974,6 +2969,11 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3006,7 +3006,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3040,7 +3040,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3264,9 +3264,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F138" sqref="E138:F138"/>
+      <selection pane="topRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -3284,20 +3284,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1" thickBot="1">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="90"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="97"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
       <c r="A2" s="75" t="s">
-        <v>752</v>
+        <v>766</v>
       </c>
       <c r="B2" s="76"/>
       <c r="C2" s="77"/>
@@ -3334,31 +3334,31 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="24">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="89" t="s">
         <v>617</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="88" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="80">
         <v>2</v>
       </c>
       <c r="D4" s="81"/>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="97" t="s">
+      <c r="H4" s="94" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.25">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="90" t="s">
         <v>618</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -3382,7 +3382,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="91" t="s">
         <v>619</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -3401,7 +3401,7 @@
       <c r="G6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="97" t="s">
+      <c r="H6" s="94" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3449,7 +3449,7 @@
       <c r="G8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="97" t="s">
+      <c r="H8" s="94" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3497,7 +3497,7 @@
       <c r="G10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="97" t="s">
+      <c r="H10" s="94" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3545,7 +3545,7 @@
       <c r="G12" s="11">
         <v>2484</v>
       </c>
-      <c r="H12" s="97" t="s">
+      <c r="H12" s="94" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3593,7 +3593,7 @@
       <c r="G14" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="97" t="s">
+      <c r="H14" s="94" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3641,7 +3641,7 @@
       <c r="G16" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="97" t="s">
+      <c r="H16" s="94" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3689,7 +3689,7 @@
       <c r="G18" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="97" t="s">
+      <c r="H18" s="94" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3737,12 +3737,12 @@
       <c r="G20" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="97" t="s">
+      <c r="H20" s="94" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="90" t="s">
         <v>634</v>
       </c>
       <c r="B21" s="22" t="s">
@@ -3769,7 +3769,7 @@
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" ht="24">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="91" t="s">
         <v>635</v>
       </c>
       <c r="B22" s="15" t="s">
@@ -3788,12 +3788,12 @@
       <c r="G22" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H22" s="97" t="s">
+      <c r="H22" s="94" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="24">
-      <c r="A23" s="93" t="s">
+      <c r="A23" s="90" t="s">
         <v>636</v>
       </c>
       <c r="B23" s="29" t="s">
@@ -3817,7 +3817,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="14.25">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="91" t="s">
         <v>637</v>
       </c>
       <c r="B24" s="18" t="s">
@@ -3836,12 +3836,12 @@
       <c r="G24" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="H24" s="97" t="s">
+      <c r="H24" s="94" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="24">
-      <c r="A25" s="93" t="s">
+      <c r="A25" s="90" t="s">
         <v>638</v>
       </c>
       <c r="B25" s="22" t="s">
@@ -3865,7 +3865,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="14.25">
-      <c r="A26" s="94" t="s">
+      <c r="A26" s="91" t="s">
         <v>639</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3884,7 +3884,7 @@
       <c r="G26" s="11">
         <v>1352</v>
       </c>
-      <c r="H26" s="97" t="s">
+      <c r="H26" s="94" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3932,7 +3932,7 @@
       <c r="G28" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H28" s="97" t="s">
+      <c r="H28" s="94" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3980,7 +3980,7 @@
       <c r="G30" s="11">
         <v>2644</v>
       </c>
-      <c r="H30" s="97" t="s">
+      <c r="H30" s="94" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4028,7 +4028,7 @@
       <c r="G32" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="H32" s="97" t="s">
+      <c r="H32" s="94" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4076,7 +4076,7 @@
       <c r="G34" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="H34" s="97" t="s">
+      <c r="H34" s="94" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4124,7 +4124,7 @@
       <c r="G36" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="H36" s="97" t="s">
+      <c r="H36" s="94" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4172,7 +4172,7 @@
       <c r="G38" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="H38" s="97" t="s">
+      <c r="H38" s="94" t="s">
         <v>178</v>
       </c>
     </row>
@@ -4220,7 +4220,7 @@
       <c r="G40" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="H40" s="97" t="s">
+      <c r="H40" s="94" t="s">
         <v>184</v>
       </c>
     </row>
@@ -4268,7 +4268,7 @@
       <c r="G42" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="H42" s="97" t="s">
+      <c r="H42" s="94" t="s">
         <v>196</v>
       </c>
     </row>
@@ -4316,7 +4316,7 @@
       <c r="G44" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="H44" s="97" t="s">
+      <c r="H44" s="94" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4364,7 +4364,7 @@
       <c r="G46" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="H46" s="97" t="s">
+      <c r="H46" s="94" t="s">
         <v>184</v>
       </c>
     </row>
@@ -4412,7 +4412,7 @@
       <c r="G48" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="H48" s="97" t="s">
+      <c r="H48" s="94" t="s">
         <v>184</v>
       </c>
     </row>
@@ -4460,7 +4460,7 @@
       <c r="G50" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="H50" s="97" t="s">
+      <c r="H50" s="94" t="s">
         <v>234</v>
       </c>
     </row>
@@ -4502,7 +4502,7 @@
       <c r="E52" s="38"/>
       <c r="F52" s="38"/>
       <c r="G52" s="11"/>
-      <c r="H52" s="97" t="s">
+      <c r="H52" s="94" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4550,7 +4550,7 @@
       <c r="G54" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="H54" s="97" t="s">
+      <c r="H54" s="94" t="s">
         <v>184</v>
       </c>
     </row>
@@ -4598,7 +4598,7 @@
       <c r="G56" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="H56" s="97" t="s">
+      <c r="H56" s="94" t="s">
         <v>255</v>
       </c>
     </row>
@@ -4646,7 +4646,7 @@
       <c r="G58" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="H58" s="97" t="s">
+      <c r="H58" s="94" t="s">
         <v>264</v>
       </c>
     </row>
@@ -4694,7 +4694,7 @@
       <c r="G60" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="H60" s="97" t="s">
+      <c r="H60" s="94" t="s">
         <v>273</v>
       </c>
     </row>
@@ -4742,7 +4742,7 @@
       <c r="G62" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="H62" s="97" t="s">
+      <c r="H62" s="94" t="s">
         <v>284</v>
       </c>
     </row>
@@ -4790,7 +4790,7 @@
       <c r="G64" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="H64" s="97" t="s">
+      <c r="H64" s="94" t="s">
         <v>294</v>
       </c>
     </row>
@@ -4838,7 +4838,7 @@
       <c r="G66" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="H66" s="97" t="s">
+      <c r="H66" s="94" t="s">
         <v>305</v>
       </c>
     </row>
@@ -4886,7 +4886,7 @@
       <c r="G68" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="H68" s="97" t="s">
+      <c r="H68" s="94" t="s">
         <v>316</v>
       </c>
     </row>
@@ -4934,7 +4934,7 @@
       <c r="G70" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="H70" s="97" t="s">
+      <c r="H70" s="94" t="s">
         <v>326</v>
       </c>
     </row>
@@ -4982,7 +4982,7 @@
       <c r="G72" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="H72" s="97" t="s">
+      <c r="H72" s="94" t="s">
         <v>336</v>
       </c>
     </row>
@@ -5030,7 +5030,7 @@
       <c r="G74" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="H74" s="97" t="s">
+      <c r="H74" s="94" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5078,7 +5078,7 @@
       <c r="G76" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="H76" s="97" t="s">
+      <c r="H76" s="94" t="s">
         <v>353</v>
       </c>
     </row>
@@ -5126,7 +5126,7 @@
       <c r="G78" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="H78" s="97" t="s">
+      <c r="H78" s="94" t="s">
         <v>362</v>
       </c>
     </row>
@@ -5174,7 +5174,7 @@
       <c r="G80" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="H80" s="97" t="s">
+      <c r="H80" s="94" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5222,7 +5222,7 @@
       <c r="G82" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="H82" s="97" t="s">
+      <c r="H82" s="94" t="s">
         <v>381</v>
       </c>
     </row>
@@ -5270,7 +5270,7 @@
       <c r="G84" s="11" t="s">
         <v>390</v>
       </c>
-      <c r="H84" s="97" t="s">
+      <c r="H84" s="94" t="s">
         <v>391</v>
       </c>
     </row>
@@ -5318,7 +5318,7 @@
       <c r="G86" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="H86" s="97" t="s">
+      <c r="H86" s="94" t="s">
         <v>403</v>
       </c>
     </row>
@@ -5366,7 +5366,7 @@
       <c r="G88" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="H88" s="97" t="s">
+      <c r="H88" s="94" t="s">
         <v>409</v>
       </c>
     </row>
@@ -5380,7 +5380,7 @@
       <c r="C89" s="27">
         <v>2</v>
       </c>
-      <c r="D89" s="95"/>
+      <c r="D89" s="92"/>
       <c r="E89" s="22" t="s">
         <v>415</v>
       </c>
@@ -5414,7 +5414,7 @@
       <c r="G90" s="11" t="s">
         <v>422</v>
       </c>
-      <c r="H90" s="97" t="s">
+      <c r="H90" s="94" t="s">
         <v>423</v>
       </c>
     </row>
@@ -5462,7 +5462,7 @@
       <c r="G92" s="11" t="s">
         <v>432</v>
       </c>
-      <c r="H92" s="97" t="s">
+      <c r="H92" s="94" t="s">
         <v>433</v>
       </c>
     </row>
@@ -5510,7 +5510,7 @@
       <c r="G94" s="17" t="s">
         <v>442</v>
       </c>
-      <c r="H94" s="97" t="s">
+      <c r="H94" s="94" t="s">
         <v>443</v>
       </c>
     </row>
@@ -5558,7 +5558,7 @@
       <c r="G96" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="H96" s="97" t="s">
+      <c r="H96" s="94" t="s">
         <v>451</v>
       </c>
     </row>
@@ -5572,7 +5572,7 @@
       <c r="C97" s="40">
         <v>3</v>
       </c>
-      <c r="D97" s="95"/>
+      <c r="D97" s="92"/>
       <c r="E97" s="22" t="s">
         <v>453</v>
       </c>
@@ -5606,7 +5606,7 @@
       <c r="G98" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="H98" s="97" t="s">
+      <c r="H98" s="94" t="s">
         <v>460</v>
       </c>
     </row>
@@ -5654,7 +5654,7 @@
       <c r="G100" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="H100" s="97" t="s">
+      <c r="H100" s="94" t="s">
         <v>460</v>
       </c>
     </row>
@@ -5702,7 +5702,7 @@
       <c r="G102" s="11" t="s">
         <v>478</v>
       </c>
-      <c r="H102" s="97" t="s">
+      <c r="H102" s="94" t="s">
         <v>479</v>
       </c>
     </row>
@@ -5750,7 +5750,7 @@
       <c r="G104" s="11" t="s">
         <v>487</v>
       </c>
-      <c r="H104" s="97" t="s">
+      <c r="H104" s="94" t="s">
         <v>488</v>
       </c>
     </row>
@@ -5798,7 +5798,7 @@
       <c r="G106" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="H106" s="97" t="s">
+      <c r="H106" s="94" t="s">
         <v>495</v>
       </c>
     </row>
@@ -5807,7 +5807,7 @@
         <v>720</v>
       </c>
       <c r="B107" s="22" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C107" s="34" t="s">
         <v>496</v>
@@ -5823,7 +5823,7 @@
         <v>499</v>
       </c>
       <c r="H107" s="65" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="15.75" customHeight="1">
@@ -5844,7 +5844,7 @@
       <c r="G108" s="11" t="s">
         <v>503</v>
       </c>
-      <c r="H108" s="97" t="s">
+      <c r="H108" s="94" t="s">
         <v>509</v>
       </c>
     </row>
@@ -5888,7 +5888,7 @@
       <c r="G110" s="11" t="s">
         <v>513</v>
       </c>
-      <c r="H110" s="97" t="s">
+      <c r="H110" s="94" t="s">
         <v>510</v>
       </c>
     </row>
@@ -6025,7 +6025,7 @@
       </c>
     </row>
     <row r="117" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A117" s="96" t="s">
+      <c r="A117" s="93" t="s">
         <v>730</v>
       </c>
       <c r="B117" s="44" t="s">
@@ -6410,13 +6410,13 @@
       <c r="C135" s="53"/>
       <c r="D135" s="53"/>
       <c r="E135" s="54" t="s">
+        <v>761</v>
+      </c>
+      <c r="F135" s="54" t="s">
         <v>762</v>
       </c>
-      <c r="F135" s="54" t="s">
+      <c r="G135" s="55" t="s">
         <v>763</v>
-      </c>
-      <c r="G135" s="55" t="s">
-        <v>764</v>
       </c>
       <c r="H135" s="68"/>
     </row>
@@ -6430,13 +6430,13 @@
       <c r="C136" s="48"/>
       <c r="D136" s="48"/>
       <c r="E136" s="49" t="s">
+        <v>758</v>
+      </c>
+      <c r="F136" s="49" t="s">
         <v>759</v>
       </c>
-      <c r="F136" s="49" t="s">
+      <c r="G136" s="50" t="s">
         <v>760</v>
-      </c>
-      <c r="G136" s="50" t="s">
-        <v>761</v>
       </c>
       <c r="H136" s="64"/>
     </row>
@@ -6450,13 +6450,13 @@
       <c r="C137" s="53"/>
       <c r="D137" s="53"/>
       <c r="E137" s="54" t="s">
+        <v>755</v>
+      </c>
+      <c r="F137" s="54" t="s">
         <v>756</v>
       </c>
-      <c r="F137" s="54" t="s">
+      <c r="G137" s="55" t="s">
         <v>757</v>
-      </c>
-      <c r="G137" s="55" t="s">
-        <v>758</v>
       </c>
       <c r="H137" s="68"/>
     </row>
@@ -6470,13 +6470,13 @@
       <c r="C138" s="71"/>
       <c r="D138" s="71"/>
       <c r="E138" s="72" t="s">
+        <v>752</v>
+      </c>
+      <c r="F138" s="72" t="s">
         <v>753</v>
       </c>
-      <c r="F138" s="72" t="s">
+      <c r="G138" s="73" t="s">
         <v>754</v>
-      </c>
-      <c r="G138" s="73" t="s">
-        <v>755</v>
       </c>
       <c r="H138" s="74"/>
     </row>

</xml_diff>